<commit_message>
update grid and acccpetance tests
</commit_message>
<xml_diff>
--- a/maven-A1/4004-F18-A1-gridv3.xlsx
+++ b/maven-A1/4004-F18-A1-gridv3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174">
   <si>
     <t>COMP4004 - Fall 2018 - Assignment 1</t>
   </si>
@@ -233,6 +233,9 @@
     <t xml:space="preserve">exactly 3 cards of the same rank </t>
   </si>
   <si>
+    <t>Stragtegy4Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">exactly 3 cards in sequence </t>
   </si>
   <si>
@@ -338,36 +341,60 @@
     <t>For either player,  detect  you are 1 card away from a royal flush and exchange that card</t>
   </si>
   <si>
-    <t>test1 2 line   AIP wins    CompareTest test1</t>
+    <t>test2 1 line   AIP wins    CompareTest1 test1</t>
   </si>
   <si>
     <t>For either player,  detect you are 1 card away from a straight flush and exchange that card</t>
   </si>
   <si>
+    <t>test2 2 line   AIP wins    CompareTest1 test2</t>
+  </si>
+  <si>
     <t>For either player,  detect you are 1 card away from a  flush and exchange that card</t>
   </si>
   <si>
+    <t>test2 16 line   AIP wins    CompareTest1 test16</t>
+  </si>
+  <si>
     <t>For either player,  detect you are 1 card away from a straight and exchange that card</t>
   </si>
   <si>
+    <t>test2 7 line   AIP wins    CompareTest1 test7</t>
+  </si>
+  <si>
     <t>For either player,   detect 3 cards of the same suit &amp; exchange other two</t>
   </si>
   <si>
+    <t>test3 1 line   AIP wins    CompareTest1 test1</t>
+  </si>
+  <si>
     <t>For either player,  detect 3 cards of the same rank &amp; exchange other two</t>
   </si>
   <si>
     <t>For either player,  detect 3 cards in sequence &amp; exchange other two</t>
   </si>
   <si>
+    <t>test3 2 line   AIP wins    CompareTest1 test2</t>
+  </si>
+  <si>
     <t>For either player,  detect two distinct pairs and exchange the other card</t>
   </si>
   <si>
+    <t>test3 3 line   AIP wins    CompareTest1 test3</t>
+  </si>
+  <si>
     <t>For either player,  detect a single pair and exchange the other 3 cards</t>
   </si>
   <si>
+    <t>test3 4 line   AIP wins    CompareTest1 test4</t>
+  </si>
+  <si>
     <t>If none of the above, then keep highest 2 and exchange 3 others</t>
   </si>
   <si>
+    <t>test3 5 line   AIP wins    CompareTest1 test5</t>
+  </si>
+  <si>
     <t>Winning</t>
   </si>
   <si>
@@ -422,24 +449,33 @@
     <t>royal flush, then the one with highest suit wins</t>
   </si>
   <si>
-    <t>test2 1 line   AIP wins    CompareTest1 test1</t>
-  </si>
-  <si>
     <t>straight flush with distinct highest card, then the one with the highest card wins</t>
   </si>
   <si>
     <t>straight flush with the same highest card, then highest suit wins</t>
   </si>
   <si>
+    <t>test2 3 line   AIP wins    CompareTest1 test3</t>
+  </si>
+  <si>
     <t>4-of-a-kind, the highest card of the 2 quadruplets wins</t>
   </si>
   <si>
+    <t>test2 4 line   AIP wins    CompareTest1 test4</t>
+  </si>
+  <si>
     <t>full house, the highest card of the 2 triplets wins</t>
   </si>
   <si>
+    <t>test2 5 line   AIP wins    CompareTest1 test5</t>
+  </si>
+  <si>
     <t>three-of-a-kind, the highest card of the 2 triplets wins</t>
   </si>
   <si>
+    <t>test2 6 line   AIP wins    CompareTest1 test6</t>
+  </si>
+  <si>
     <t xml:space="preserve">two straights with the same rank for their highest card, then highest suit </t>
   </si>
   <si>
@@ -449,37 +485,61 @@
     <t>two straights with distinct highest card, then highest card wins</t>
   </si>
   <si>
+    <t>test2 8 line   AIP wins    CompareTest1 test8</t>
+  </si>
+  <si>
     <t xml:space="preserve">two pairs with the same highest pair for each participant, </t>
   </si>
   <si>
     <t xml:space="preserve">   then highest suit of this highest pair wins</t>
   </si>
   <si>
+    <t>test2 9 line   AIP wins    CompareTest1 test9</t>
+  </si>
+  <si>
     <t>two pairs, with distinct highest pairs for the 2 participants, then highest pair wins</t>
   </si>
   <si>
+    <t>test2 10 line   AIP wins    CompareTest1 test10</t>
+  </si>
+  <si>
     <t>one pair, with both of these pairs of equal rank, then highest suit of these pairs wins</t>
   </si>
   <si>
+    <t>test2 11 line   AIP wins    CompareTest1 test11</t>
+  </si>
+  <si>
     <t xml:space="preserve">one pair, with distinct-ranked pairs for the 2 participants, </t>
   </si>
   <si>
     <t xml:space="preserve">    then pair with highest card wins</t>
   </si>
   <si>
+    <t>test2 12 line   AIP wins    CompareTest1 test12</t>
+  </si>
+  <si>
     <t>high card hand with same rank for the highest card of each participant</t>
   </si>
   <si>
     <t xml:space="preserve">  then highest suit of the highest card win</t>
   </si>
   <si>
+    <t>test2 13 line   AIP wins    CompareTest1 test13</t>
+  </si>
+  <si>
     <t>high card hand with distinct highest card for each participant</t>
   </si>
   <si>
     <t xml:space="preserve">  then highest ranked card wins</t>
   </si>
   <si>
+    <t>test2 14 line   AIP wins    CompareTest1 test14</t>
+  </si>
+  <si>
     <t>flush, and the same rank for each of their 5 cards, then highest suit of highest card wins</t>
+  </si>
+  <si>
+    <t>test2 15 line   AIP wins    CompareTest1 test15</t>
   </si>
   <si>
     <t>flush, and the same rank for each of their 4 highest cards, then highest rank of 5th card wins</t>
@@ -1637,8 +1697,8 @@
   <sheetPr/>
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -2128,7 +2188,7 @@
         <v>54</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31">
@@ -2136,7 +2196,9 @@
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -2144,7 +2206,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>16</v>
@@ -2156,7 +2218,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2165,10 +2227,10 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33">
@@ -2176,7 +2238,9 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -2184,7 +2248,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>16</v>
@@ -2196,7 +2260,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2208,13 +2272,13 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>16</v>
@@ -2227,7 +2291,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>16</v>
@@ -2239,7 +2303,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>20</v>
@@ -2251,7 +2315,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>16</v>
@@ -2266,13 +2330,13 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C42"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>20</v>
@@ -2288,12 +2352,12 @@
     </row>
     <row r="44" spans="5:5">
       <c r="E44" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>16</v>
@@ -2303,7 +2367,7 @@
         <v>0.5</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2316,7 +2380,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>16</v>
@@ -2326,7 +2390,7 @@
         <v>0.5</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2339,7 +2403,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>16</v>
@@ -2349,7 +2413,7 @@
         <v>0.5</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2362,7 +2426,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>16</v>
@@ -2372,7 +2436,7 @@
         <v>0.5</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -2385,7 +2449,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>16</v>
@@ -2395,7 +2459,7 @@
         <v>0.5</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2408,7 +2472,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>16</v>
@@ -2418,7 +2482,7 @@
         <v>0.5</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -2431,7 +2495,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>16</v>
@@ -2441,7 +2505,7 @@
         <v>0.5</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -2454,16 +2518,18 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52">
         <v>0.5</v>
       </c>
-      <c r="E52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2475,16 +2541,18 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53">
         <v>0.5</v>
       </c>
-      <c r="E53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -2496,16 +2564,18 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54">
         <v>0.5</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2517,16 +2587,18 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55">
         <v>0.5</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -2538,10 +2610,10 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56">
@@ -2559,16 +2631,18 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57">
         <v>0.5</v>
       </c>
-      <c r="E57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -2580,16 +2654,18 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58">
         <v>0.5</v>
       </c>
-      <c r="E58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -2601,16 +2677,18 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59">
         <v>0.5</v>
       </c>
-      <c r="E59" s="3"/>
+      <c r="E59" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -2622,16 +2700,18 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60">
         <v>0.5</v>
       </c>
-      <c r="E60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -2646,13 +2726,13 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C62"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>16</v>
@@ -2662,7 +2742,7 @@
         <v>0.25</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2676,7 +2756,7 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>16</v>
@@ -2686,7 +2766,7 @@
         <v>0.5</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -2700,7 +2780,7 @@
     </row>
     <row r="65" spans="1:13">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>16</v>
@@ -2710,7 +2790,7 @@
         <v>0.25</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -2724,7 +2804,7 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>16</v>
@@ -2734,7 +2814,7 @@
         <v>0.25</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -2748,7 +2828,7 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>16</v>
@@ -2758,7 +2838,7 @@
         <v>0.25</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -2772,7 +2852,7 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>16</v>
@@ -2782,7 +2862,7 @@
         <v>0.25</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -2796,7 +2876,7 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>16</v>
@@ -2806,7 +2886,7 @@
         <v>0.25</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -2820,7 +2900,7 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>16</v>
@@ -2830,7 +2910,7 @@
         <v>0.25</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2844,7 +2924,7 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>16</v>
@@ -2854,7 +2934,7 @@
         <v>0.25</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2871,19 +2951,19 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C73"/>
       <c r="M73" s="8"/>
     </row>
     <row r="74" s="1" customFormat="1" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>16</v>
@@ -2893,7 +2973,7 @@
         <v>0.5</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -2906,16 +2986,18 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76">
         <v>0.5</v>
       </c>
-      <c r="E76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -2927,16 +3009,18 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77">
         <v>0.5</v>
       </c>
-      <c r="E77" s="3"/>
+      <c r="E77" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
@@ -2948,16 +3032,18 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78">
         <v>0.5</v>
       </c>
-      <c r="E78" s="3"/>
+      <c r="E78" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -2969,16 +3055,18 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79">
         <v>0.5</v>
       </c>
-      <c r="E79" s="3"/>
+      <c r="E79" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -2990,16 +3078,18 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80">
         <v>0.5</v>
       </c>
-      <c r="E80" s="3"/>
+      <c r="E80" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
@@ -3011,22 +3101,24 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C81"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82">
         <v>0.5</v>
       </c>
-      <c r="E82" s="3"/>
+      <c r="E82" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
@@ -3038,16 +3130,18 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83">
         <v>0.5</v>
       </c>
-      <c r="E83" s="3"/>
+      <c r="E83" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
@@ -3059,7 +3153,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B84" s="2"/>
       <c r="D84" s="2"/>
@@ -3071,16 +3165,18 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85">
         <v>0.5</v>
       </c>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -3092,16 +3188,18 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86">
         <v>0.5</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
@@ -3111,29 +3209,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>135</v>
+      </c>
+      <c r="B87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89">
         <v>0.5</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
@@ -3145,21 +3251,23 @@
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91">
         <v>0.5</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
@@ -3171,21 +3279,23 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93">
         <v>0.5</v>
       </c>
-      <c r="E93" s="3"/>
+      <c r="E93" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
@@ -3197,16 +3307,18 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94">
         <v>0.5</v>
       </c>
-      <c r="E94" s="3"/>
+      <c r="E94" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -3218,7 +3330,7 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>20</v>
@@ -3239,12 +3351,12 @@
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>20</v>
@@ -3265,12 +3377,12 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>20</v>
@@ -3291,7 +3403,7 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="8" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -3308,7 +3420,7 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="8" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>20</v>
@@ -3334,7 +3446,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="13" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C103" s="10">
         <f>SUM(C8:C101)</f>
@@ -3351,13 +3463,13 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C105"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="14" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>20</v>
@@ -3378,7 +3490,7 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="14" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B107" s="11" t="s">
         <v>20</v>
@@ -3399,7 +3511,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="13" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="10">
@@ -3413,12 +3525,12 @@
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112">
@@ -3427,7 +3539,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113">
@@ -3436,7 +3548,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="C114" s="7"/>
       <c r="D114">
@@ -3445,7 +3557,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115">
@@ -3454,7 +3566,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="C116" s="7"/>
       <c r="D116">
@@ -3463,19 +3575,19 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C117" s="7"/>
       <c r="D117">
         <v>-40</v>
       </c>
       <c r="E117" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="C118" s="7"/>
       <c r="D118">
@@ -3484,7 +3596,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C119" s="7"/>
       <c r="D119">
@@ -3493,7 +3605,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120">
@@ -3502,7 +3614,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121">
@@ -3511,7 +3623,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122">
@@ -3520,7 +3632,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="15" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="C124" s="16">
         <f>C108-SUM(C112:C120)</f>

</xml_diff>

<commit_message>
pass suit and rank test
</commit_message>
<xml_diff>
--- a/maven-A1/4004-F18-A1-gridv3.xlsx
+++ b/maven-A1/4004-F18-A1-gridv3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9947" tabRatio="500"/>
+    <workbookView windowWidth="28695" windowHeight="12630" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178">
   <si>
     <t>COMP4004 - Fall 2018 - Assignment 1</t>
   </si>
@@ -22,7 +22,13 @@
     <t>First Name</t>
   </si>
   <si>
+    <t>yuhua</t>
+  </si>
+  <si>
     <t>Last Name</t>
+  </si>
+  <si>
+    <t>wang</t>
   </si>
   <si>
     <t>Student #</t>
@@ -106,67 +112,70 @@
     <t>You have at least one test that shows suits are correctly ranked</t>
   </si>
   <si>
+    <t>SuitTest</t>
+  </si>
+  <si>
+    <t>You have at least one test that shows cards are correctly ranked</t>
+  </si>
+  <si>
+    <t>names of relevant  Junit tests that run (tests that do not run are worth 0)</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect a royal flush whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>RoyalFlushTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect a straight flush whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>StraightTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect 4-of-a-kind whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>FOAKTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect a full house whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>FullHouseTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect a flush whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>FlushTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect a straight whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect 3-of-a-kind whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>TOAKTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect two pairs whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>TwoPairTest</t>
+  </si>
+  <si>
+    <t>You have tests that show you can detect a pair whatever the order of the cards</t>
+  </si>
+  <si>
+    <t>PairTest</t>
+  </si>
+  <si>
+    <t>You have tests that show detecting what's in a hand is independent of whose hand it is</t>
+  </si>
+  <si>
     <t>yes/no</t>
-  </si>
-  <si>
-    <t>You have at least one test that shows cards are correctly ranked</t>
-  </si>
-  <si>
-    <t>names of relevant  Junit tests that run (tests that do not run are worth 0)</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect a royal flush whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>RoyalFlushTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect a straight flush whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>StraightTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect 4-of-a-kind whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>FOAKTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect a full house whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>FullHouseTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect a flush whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>FlushTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect a straight whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect 3-of-a-kind whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>TOAKTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect two pairs whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>TwoPairTest</t>
-  </si>
-  <si>
-    <t>You have tests that show you can detect a pair whatever the order of the cards</t>
-  </si>
-  <si>
-    <t>PairTest</t>
-  </si>
-  <si>
-    <t>You have tests that show detecting what's in a hand is independent of whose hand it is</t>
   </si>
   <si>
     <t xml:space="preserve">You have tests that show what's detected in AIP's hand is independent </t>
@@ -545,6 +554,9 @@
     <t>flush, and the same rank for each of their 4 highest cards, then highest rank of 5th card wins</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>flush, and the same rank for their 3 highest cards,</t>
   </si>
   <si>
@@ -625,12 +637,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -677,7 +689,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,6 +718,43 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -698,7 +762,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -714,68 +816,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -789,28 +839,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="12"/>
@@ -859,7 +887,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,37 +983,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -913,43 +1043,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -961,85 +1061,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1053,11 +1081,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1073,6 +1122,35 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1100,195 +1178,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1315,7 +1349,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
     <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
@@ -1326,43 +1360,45 @@
     <cellStyle name="差" xfId="7" builtinId="27"/>
     <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
     <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="百分比" xfId="10" builtinId="5"/>
-    <cellStyle name="注释" xfId="11" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="12" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="13" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11"/>
-    <cellStyle name="标题" xfId="15" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="17" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="18" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="19" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="20" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="21" builtinId="44"/>
-    <cellStyle name="输出" xfId="22" builtinId="21"/>
-    <cellStyle name="计算" xfId="23" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="24" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="25" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="26" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="27" builtinId="24"/>
-    <cellStyle name="汇总" xfId="28" builtinId="25"/>
-    <cellStyle name="好" xfId="29" builtinId="26"/>
-    <cellStyle name="适中" xfId="30" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="31" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="32" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="33" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="34" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="35" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="36" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="37" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="38" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="39" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="40" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="42" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="43" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="44" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="45" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="46" builtinId="52"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
@@ -1697,11 +1733,11 @@
   <sheetPr/>
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="115.641666666667" customWidth="1"/>
     <col min="3" max="3" width="10.8333333333333" style="2"/>
@@ -1714,19 +1750,25 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>100979805</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
     </row>
@@ -1735,53 +1777,53 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8">
@@ -1790,10 +1832,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9">
@@ -1802,49 +1844,52 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13">
@@ -1853,7 +1898,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1862,10 +1907,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14">
@@ -1874,7 +1919,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1883,10 +1928,10 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15">
@@ -1895,7 +1940,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1904,10 +1949,10 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16">
@@ -1916,7 +1961,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1925,10 +1970,10 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17">
@@ -1937,7 +1982,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1946,10 +1991,10 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18">
@@ -1958,7 +2003,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1967,10 +2012,10 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19">
@@ -1979,7 +2024,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1988,10 +2033,10 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20">
@@ -2000,7 +2045,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -2009,10 +2054,10 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21">
@@ -2021,7 +2066,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -2030,10 +2075,10 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22">
@@ -2049,16 +2094,16 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24">
@@ -2074,16 +2119,16 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26">
@@ -2092,7 +2137,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -2101,10 +2146,10 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27">
@@ -2113,7 +2158,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -2122,10 +2167,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28">
@@ -2134,7 +2179,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -2143,10 +2188,10 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29">
@@ -2155,7 +2200,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -2164,10 +2209,10 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30">
@@ -2176,7 +2221,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2185,10 +2230,10 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31">
@@ -2197,7 +2242,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -2206,10 +2251,10 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32">
@@ -2218,7 +2263,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2227,10 +2272,10 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33">
@@ -2239,7 +2284,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -2248,10 +2293,10 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34">
@@ -2260,7 +2305,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2272,16 +2317,16 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C36"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37">
@@ -2291,10 +2336,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38">
@@ -2303,10 +2348,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39">
@@ -2315,10 +2360,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40">
@@ -2330,16 +2375,16 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C42"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C43" s="10">
         <f>SUM(J45:J101)</f>
@@ -2352,22 +2397,22 @@
     </row>
     <row r="44" spans="5:5">
       <c r="E44" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45">
         <v>0.5</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2380,17 +2425,17 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46">
         <v>0.5</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2403,17 +2448,17 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47">
         <v>0.5</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2426,17 +2471,17 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48">
         <v>0.5</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -2449,17 +2494,17 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49">
         <v>0.5</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2472,17 +2517,17 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50">
         <v>0.5</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -2495,17 +2540,17 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51">
         <v>0.5</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -2518,17 +2563,17 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52">
         <v>0.5</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -2541,17 +2586,17 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53">
         <v>0.5</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -2564,17 +2609,17 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54">
         <v>0.5</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -2587,17 +2632,17 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55">
         <v>0.5</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -2610,10 +2655,10 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56">
@@ -2631,17 +2676,17 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57">
         <v>0.5</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -2654,17 +2699,17 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58">
         <v>0.5</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2677,17 +2722,17 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59">
         <v>0.5</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -2700,17 +2745,17 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60">
         <v>0.5</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -2726,23 +2771,23 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C62"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63">
         <v>0.25</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2756,17 +2801,17 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64">
         <v>0.5</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -2780,17 +2825,17 @@
     </row>
     <row r="65" spans="1:13">
       <c r="A65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65">
         <v>0.25</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -2804,17 +2849,17 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66">
         <v>0.25</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -2828,17 +2873,17 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67">
         <v>0.25</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -2852,17 +2897,17 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68">
         <v>0.25</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -2876,17 +2921,17 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69">
         <v>0.25</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -2900,17 +2945,17 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70">
         <v>0.25</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2924,17 +2969,17 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71">
         <v>0.25</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2951,29 +2996,29 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C73"/>
       <c r="M73" s="8"/>
     </row>
     <row r="74" s="1" customFormat="1" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75">
         <v>0.5</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -2986,17 +3031,17 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76">
         <v>0.5</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -3009,17 +3054,17 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77">
         <v>0.5</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -3032,17 +3077,17 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78">
         <v>0.5</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -3055,17 +3100,17 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79">
         <v>0.5</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -3078,17 +3123,17 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80">
         <v>0.5</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -3101,23 +3146,23 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C81"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82">
         <v>0.5</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -3130,17 +3175,17 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83">
         <v>0.5</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -3153,7 +3198,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B84" s="2"/>
       <c r="D84" s="2"/>
@@ -3165,17 +3210,17 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85">
         <v>0.5</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -3188,17 +3233,17 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86">
         <v>0.5</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -3211,34 +3256,34 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E87" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89">
         <v>0.5</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -3251,22 +3296,22 @@
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91">
         <v>0.5</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -3279,22 +3324,22 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93">
         <v>0.5</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -3307,17 +3352,17 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94">
         <v>0.5</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -3330,10 +3375,10 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95">
@@ -3351,15 +3396,15 @@
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97">
@@ -3377,15 +3422,15 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
+        <v>156</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99">
@@ -3403,7 +3448,7 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -3420,10 +3465,10 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="8" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C101" s="12"/>
       <c r="D101">
@@ -3446,7 +3491,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="13" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C103" s="10">
         <f>SUM(C8:C101)</f>
@@ -3463,16 +3508,16 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C105"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="14" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C106" s="12"/>
       <c r="D106">
@@ -3490,10 +3535,10 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="14" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C107" s="12"/>
       <c r="D107">
@@ -3511,7 +3556,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="13" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="10">
@@ -3525,12 +3570,12 @@
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112">
@@ -3539,7 +3584,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113">
@@ -3548,7 +3593,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C114" s="7"/>
       <c r="D114">
@@ -3557,7 +3602,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115">
@@ -3566,7 +3611,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C116" s="7"/>
       <c r="D116">
@@ -3575,19 +3620,19 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C117" s="7"/>
       <c r="D117">
         <v>-40</v>
       </c>
       <c r="E117" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C118" s="7"/>
       <c r="D118">
@@ -3596,7 +3641,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C119" s="7"/>
       <c r="D119">
@@ -3605,7 +3650,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120">
@@ -3614,7 +3659,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121">
@@ -3623,7 +3668,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122">
@@ -3632,7 +3677,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="15" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C124" s="16">
         <f>C108-SUM(C112:C120)</f>

</xml_diff>